<commit_message>
Se agrega el metodo propio de testng para validacion de la prueba, esta validación se realiza en el método takeScreenShotOnFailure despues de la ejecución de la prueba.
</commit_message>
<xml_diff>
--- a/DataTestPractice.xlsx
+++ b/DataTestPractice.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
+    <workbookView windowHeight="3525" windowWidth="12255" xWindow="0" yWindow="2445"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" r:id="rId1" sheetId="1"/>
     <sheet name="Hoja2" r:id="rId2" sheetId="2"/>
     <sheet name="Hoja3" r:id="rId3" sheetId="3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>usuario</t>
   </si>
@@ -30,19 +31,22 @@
     <t>wo123</t>
   </si>
   <si>
+    <t>Articulo</t>
+  </si>
+  <si>
+    <t>ResultadoPrueba</t>
+  </si>
+  <si>
+    <t>Printed Summer Dress</t>
+  </si>
+  <si>
     <t>Faded Short Sleeve T-shirts</t>
   </si>
   <si>
-    <t>Articulo</t>
-  </si>
-  <si>
-    <t>ResultadoPrueba</t>
+    <t>Failed</t>
   </si>
   <si>
     <t>Passed</t>
-  </si>
-  <si>
-    <t>Printed Summer Dress</t>
   </si>
 </sst>
 </file>
@@ -95,14 +99,7 @@
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -142,8 +139,8 @@
   </dxfs>
   <tableStyles count="1" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2">
     <tableStyle count="2" name="MySqlDefault" pivot="0" table="0">
-      <tableStyleElement dxfId="4" type="wholeTable"/>
-      <tableStyleElement dxfId="3" type="headerRow"/>
+      <tableStyleElement dxfId="3" type="wholeTable"/>
+      <tableStyleElement dxfId="2" type="headerRow"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -441,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,10 +461,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -478,10 +475,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -492,7 +489,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3"/>
     </row>
@@ -501,10 +498,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule dxfId="0" operator="equal" priority="2" type="cellIs">
+    <cfRule dxfId="1" operator="equal" priority="2" type="cellIs">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule dxfId="1" operator="equal" priority="1" type="cellIs">
+    <cfRule dxfId="0" operator="equal" priority="1" type="cellIs">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>